<commit_message>
Updated Add Customer Test
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/AddCustomer.xlsx
+++ b/src/test/resources/testData/AddCustomer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\eclipse-workspace\XYZBankAutomationFramework\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941B090D-AD2D-438D-9E6B-74AE359B05AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E78F301-14AA-4907-A2F6-1F48CD5F7E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29790" yWindow="1200" windowWidth="25440" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33135" yWindow="3195" windowWidth="25440" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>TestName</t>
   </si>
@@ -61,6 +61,45 @@
   </si>
   <si>
     <t>PostCode</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>nullValue</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>AddCustomerError1</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Adds Customer No Errors</t>
+  </si>
+  <si>
+    <t>Mandatory Field Error PostCode pops up</t>
+  </si>
+  <si>
+    <t>Mandatory Field Error LastName pops up</t>
+  </si>
+  <si>
+    <t>AddCustomerError2</t>
+  </si>
+  <si>
+    <t>AddCustomerError3</t>
+  </si>
+  <si>
+    <t>Gary</t>
+  </si>
+  <si>
+    <t>Mandatory Field Error FirstName pops up</t>
   </si>
 </sst>
 </file>
@@ -385,15 +424,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,13 +452,19 @@
       <c r="E1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -426,13 +475,19 @@
       <c r="E2">
         <v>14110</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -443,13 +498,78 @@
       <c r="E3">
         <v>10011</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>1011</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>1011</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>